<commit_message>
fixed data provider issues
</commit_message>
<xml_diff>
--- a/test/akhan/data/akhan-combined-test-data.xlsx
+++ b/test/akhan/data/akhan-combined-test-data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="LoginData" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,32 +397,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>testId</v>
+        <v>testCase</v>
       </c>
       <c r="B1" t="str">
+        <v>testType</v>
+      </c>
+      <c r="C1" t="str">
         <v>username</v>
       </c>
-      <c r="C1" t="str">
+      <c r="D1" t="str">
         <v>password</v>
       </c>
-      <c r="D1" t="str">
-        <v>expectedWelcomeMessage</v>
-      </c>
       <c r="E1" t="str">
-        <v>executeTest</v>
+        <v>module</v>
       </c>
       <c r="F1" t="str">
-        <v>priority</v>
+        <v>expectedResult</v>
       </c>
       <c r="G1" t="str">
+        <v>executeFlag</v>
+      </c>
+      <c r="H1" t="str">
         <v>environment</v>
+      </c>
+      <c r="I1" t="str">
+        <v>priority_x000d_</v>
       </c>
     </row>
     <row r="2">
@@ -433,19 +439,22 @@
         <v>login</v>
       </c>
       <c r="C2" t="str">
-        <v>passwd</v>
+        <v>Admin</v>
       </c>
       <c r="D2" t="str">
-        <v>Welcome to AKHAN</v>
-      </c>
-      <c r="E2" t="str">
-        <v>true</v>
+        <v>admin123</v>
       </c>
       <c r="F2" t="str">
-        <v>high</v>
-      </c>
-      <c r="G2" t="str">
-        <v>SIT</v>
+        <v>Login successful</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="str">
+        <v>QA</v>
+      </c>
+      <c r="I2" t="str">
+        <v>high_x000d_</v>
       </c>
     </row>
     <row r="3">
@@ -453,22 +462,25 @@
         <v>TC501-2</v>
       </c>
       <c r="B3" t="str">
-        <v>testuser1</v>
+        <v>login</v>
       </c>
       <c r="C3" t="str">
-        <v>testpass1</v>
+        <v>testuser</v>
       </c>
       <c r="D3" t="str">
-        <v>Welcome Test User 1</v>
-      </c>
-      <c r="E3" t="str">
-        <v>true</v>
+        <v>test123</v>
       </c>
       <c r="F3" t="str">
-        <v>medium</v>
-      </c>
-      <c r="G3" t="str">
-        <v>SIT</v>
+        <v>Login successful</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="str">
+        <v>QA</v>
+      </c>
+      <c r="I3" t="str">
+        <v>high_x000d_</v>
       </c>
     </row>
     <row r="4">
@@ -476,50 +488,352 @@
         <v>TC501-3</v>
       </c>
       <c r="B4" t="str">
-        <v>testuser2</v>
+        <v>login</v>
       </c>
       <c r="C4" t="str">
-        <v>testpass2</v>
+        <v>manager</v>
       </c>
       <c r="D4" t="str">
-        <v>Welcome Test User 2</v>
-      </c>
-      <c r="E4" t="str">
-        <v>true</v>
+        <v>manager123</v>
       </c>
       <c r="F4" t="str">
-        <v>low</v>
-      </c>
-      <c r="G4" t="str">
-        <v>SIT</v>
+        <v>Login successful</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="str">
+        <v>QA</v>
+      </c>
+      <c r="I4" t="str">
+        <v>medium_x000d_</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>TC501-4</v>
+        <v>TC503-1</v>
       </c>
       <c r="B5" t="str">
-        <v>admin</v>
-      </c>
-      <c r="C5" t="str">
-        <v>admin123</v>
-      </c>
-      <c r="D5" t="str">
-        <v>Welcome Administrator</v>
+        <v>navigation</v>
       </c>
       <c r="E5" t="str">
-        <v>false</v>
+        <v>Admin</v>
       </c>
       <c r="F5" t="str">
-        <v>high</v>
-      </c>
-      <c r="G5" t="str">
-        <v>UAT</v>
+        <v>Admin page</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="str">
+        <v>QA</v>
+      </c>
+      <c r="I5" t="str">
+        <v>high_x000d_</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>TC503-2</v>
+      </c>
+      <c r="B6" t="str">
+        <v>navigation</v>
+      </c>
+      <c r="E6" t="str">
+        <v>PIM</v>
+      </c>
+      <c r="F6" t="str">
+        <v>PIM page</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="str">
+        <v>QA</v>
+      </c>
+      <c r="I6" t="str">
+        <v>high_x000d_</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>TC503-3</v>
+      </c>
+      <c r="B7" t="str">
+        <v>navigation</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Leave</v>
+      </c>
+      <c r="F7" t="str">
+        <v>Leave page</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="str">
+        <v>QA</v>
+      </c>
+      <c r="I7" t="str">
+        <v>medium_x000d_</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>TC503-4</v>
+      </c>
+      <c r="B8" t="str">
+        <v>navigation</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Time</v>
+      </c>
+      <c r="F8" t="str">
+        <v>Time page</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="str">
+        <v>QA</v>
+      </c>
+      <c r="I8" t="str">
+        <v>medium_x000d_</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>TC503-5</v>
+      </c>
+      <c r="B9" t="str">
+        <v>navigation</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Recruitment</v>
+      </c>
+      <c r="F9" t="str">
+        <v>Recruitment page</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="str">
+        <v>QA</v>
+      </c>
+      <c r="I9" t="str">
+        <v>medium_x000d_</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>TC503-6</v>
+      </c>
+      <c r="B10" t="str">
+        <v>navigation</v>
+      </c>
+      <c r="E10" t="str">
+        <v>My Info</v>
+      </c>
+      <c r="F10" t="str">
+        <v>My Info page</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" t="str">
+        <v>QA</v>
+      </c>
+      <c r="I10" t="str">
+        <v>low_x000d_</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>TC503-7</v>
+      </c>
+      <c r="B11" t="str">
+        <v>navigation</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Performance</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Performance page</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="str">
+        <v>QA</v>
+      </c>
+      <c r="I11" t="str">
+        <v>low_x000d_</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>TC503-8</v>
+      </c>
+      <c r="B12" t="str">
+        <v>navigation</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Dashboard</v>
+      </c>
+      <c r="F12" t="str">
+        <v>Dashboard page</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="str">
+        <v>QA</v>
+      </c>
+      <c r="I12" t="str">
+        <v>high_x000d_</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>TC503-9</v>
+      </c>
+      <c r="B13" t="str">
+        <v>navigation</v>
+      </c>
+      <c r="E13" t="str">
+        <v>Directory</v>
+      </c>
+      <c r="F13" t="str">
+        <v>Directory page</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="str">
+        <v>QA</v>
+      </c>
+      <c r="I13" t="str">
+        <v>low_x000d_</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>TC503-10</v>
+      </c>
+      <c r="B14" t="str">
+        <v>navigation</v>
+      </c>
+      <c r="E14" t="str">
+        <v>Maintenance</v>
+      </c>
+      <c r="F14" t="str">
+        <v>Maintenance page</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="str">
+        <v>QA</v>
+      </c>
+      <c r="I14" t="str">
+        <v>low_x000d_</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>TC503-11</v>
+      </c>
+      <c r="B15" t="str">
+        <v>navigation</v>
+      </c>
+      <c r="E15" t="str">
+        <v>Buzz</v>
+      </c>
+      <c r="F15" t="str">
+        <v>Buzz page</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="str">
+        <v>QA</v>
+      </c>
+      <c r="I15" t="str">
+        <v>low_x000d_</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>TC502-1</v>
+      </c>
+      <c r="B16" t="str">
+        <v>menu-verify</v>
+      </c>
+      <c r="E16" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="F16" t="str">
+        <v>Admin menu visible</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="str">
+        <v>QA</v>
+      </c>
+      <c r="I16" t="str">
+        <v>medium_x000d_</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>TC502-2</v>
+      </c>
+      <c r="B17" t="str">
+        <v>menu-verify</v>
+      </c>
+      <c r="E17" t="str">
+        <v>PIM</v>
+      </c>
+      <c r="F17" t="str">
+        <v>PIM menu visible</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="str">
+        <v>QA</v>
+      </c>
+      <c r="I17" t="str">
+        <v>medium_x000d_</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>TC502-3</v>
+      </c>
+      <c r="B18" t="str">
+        <v>menu-verify</v>
+      </c>
+      <c r="E18" t="str">
+        <v>Leave</v>
+      </c>
+      <c r="F18" t="str">
+        <v>Leave menu visible</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="str">
+        <v>QA</v>
+      </c>
+      <c r="I18" t="str">
+        <v>medium</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I18"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>